<commit_message>
pass/fail status is added
</commit_message>
<xml_diff>
--- a/fifo/doc/syn_fifo_checkpoint.xlsx
+++ b/fifo/doc/syn_fifo_checkpoint.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="128">
   <si>
     <t>Revision Information</t>
   </si>
@@ -86,7 +86,13 @@
     <t>Result</t>
   </si>
   <si>
+    <t>Note</t>
+  </si>
+  <si>
     <t>Register</t>
+  </si>
+  <si>
+    <t>Max is double of FIFO_ENTRIES</t>
   </si>
   <si>
     <t xml:space="preserve">AF/AE offset (X) </t>
@@ -155,15 +161,37 @@
 6. check DATA OUT</t>
   </si>
   <si>
-    <t>Check simultaneously write/read data</t>
+    <t>Check swap write/read data</t>
   </si>
   <si>
     <t>1. wait RESET
 2. set DATA IN
 3. set WR is high
 4. set RD is high
-5. repeat step 2
+5. repeat step 2 with 3*depth times
 6. check DATA OUT</t>
+  </si>
+  <si>
+    <t>Check simultaneously write/read data</t>
+  </si>
+  <si>
+    <t>1. wait RESET
+2. write first data into fifo
+3. simultaneously write and read data
+4. repeat step 2 with 2*depth times
+5. check DATA OUT</t>
+  </si>
+  <si>
+    <t>tc_12</t>
+  </si>
+  <si>
+    <t>syn_fifo_tc_12</t>
+  </si>
+  <si>
+    <t>syn_fifo_tc_12.sv</t>
+  </si>
+  <si>
+    <t>the delay time of sys_rclk in system_signals should be modify to #10  before this testcase run</t>
   </si>
   <si>
     <t>Check write full data when readed data</t>
@@ -205,7 +233,7 @@
     <t>1. wait RESET
 2. set DATA IN
 3. set WR is high
-4. repeat step 2 with depth/2 times
+4. repeat step 2 with 2*depth times
 5. check half-full flag</t>
   </si>
   <si>
@@ -238,7 +266,7 @@
 5. check full flag</t>
   </si>
   <si>
-    <t>Check full flag when third full fifo</t>
+    <t>Check full flag when fourth full fifo</t>
   </si>
   <si>
     <t>1. wait RESET
@@ -248,23 +276,13 @@
 5. check full flag</t>
   </si>
   <si>
-    <t>Check full flag when fourth full fifo</t>
-  </si>
-  <si>
-    <t>1. wait RESET
-2. set DATA IN
-3. set WR is high
-4. repeat step 2 with 4 x depth times
-5. check full flag</t>
-  </si>
-  <si>
     <t>Check read empty data</t>
   </si>
   <si>
     <t>1. wait RESET
 2. set RD is high
 3. wait
-4. check DATA OUT is X value</t>
+4. check DATA OUT is X value and read pointer is zero</t>
   </si>
   <si>
     <t>tc_05</t>
@@ -369,29 +387,23 @@
 5. check DATA OUT</t>
   </si>
   <si>
-    <t>Check multi-level synchronus of full flag in reset mode</t>
-  </si>
-  <si>
-    <t>1. RESET is triggered
-2. wait after two write clock
-3. check full flag</t>
-  </si>
-  <si>
-    <t>tc_08</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_08</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_08.sv</t>
-  </si>
-  <si>
-    <t>Check multi-level synchronus of empty flag in reset mode</t>
-  </si>
-  <si>
-    <t>1. RESET is triggered
-2. wait after three read clock
-3. check empty flag</t>
+    <t>Check multi-level synchronous of full flag</t>
+  </si>
+  <si>
+    <t>1. wait RESET 
+2. write first full data
+3. read first data
+4. wait after two write clock
+5. check full flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check multi-level synchronous of empty flag </t>
+  </si>
+  <si>
+    <t>1. wait RESET 
+2. write first data
+3. wait after three read clock
+4. check empty flag</t>
   </si>
   <si>
     <t>Corner Case</t>
@@ -406,13 +418,13 @@
 4. check full flag</t>
   </si>
   <si>
-    <t>tc_09</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_09</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_09.sv</t>
+    <t>tc_08</t>
+  </si>
+  <si>
+    <t>syn_fifo_tc_08</t>
+  </si>
+  <si>
+    <t>syn_fifo_tc_08.sv</t>
   </si>
   <si>
     <t>1. wait RESET
@@ -428,15 +440,6 @@
 2. w_pointer and r_pointer are assigned value: 0
 3. wait and set w_pointer is max/4
 4. check hlaf-full flag</t>
-  </si>
-  <si>
-    <t>tc_10</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_10</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_10.sv</t>
   </si>
   <si>
     <t>1. wait RESET
@@ -471,13 +474,13 @@
 9. check full flag</t>
   </si>
   <si>
-    <t>tc_11</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_11</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_11.sv</t>
+    <t>tc_09</t>
+  </si>
+  <si>
+    <t>syn_fifo_tc_09</t>
+  </si>
+  <si>
+    <t>syn_fifo_tc_09.sv</t>
   </si>
   <si>
     <t>Check upexpected stop of read data</t>
@@ -491,7 +494,7 @@
 9. check empty flag</t>
   </si>
   <si>
-    <t>Check empty flag when r_prointer is assigned  values</t>
+    <t>Check empty flag when r_prointer is assigned  a same values</t>
   </si>
   <si>
     <t>1. wait RESET
@@ -500,13 +503,13 @@
 4. check empty flag</t>
   </si>
   <si>
-    <t>tc_12</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_12</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_12.sv</t>
+    <t>tc_10</t>
+  </si>
+  <si>
+    <t>syn_fifo_tc_10</t>
+  </si>
+  <si>
+    <t>syn_fifo_tc_10.sv</t>
   </si>
   <si>
     <t>1. w_pointer and r_pointer is assigned value: 0
@@ -523,15 +526,6 @@
 4. check Af/AE flag</t>
   </si>
   <si>
-    <t>tc_13</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_13</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_13.sv</t>
-  </si>
-  <si>
     <t>1. w_pointer and r_pointer are assigned value: max
 2. wait and r_pointer is assigned respectively: X, X-1, max-X-1, max-X-2
 3. check Af/AE flag</t>
@@ -544,39 +538,29 @@
   </si>
   <si>
     <t>1. wait RESET
-2. set DATA IN and WR is high
-3. repeat step 2 with depth times
-4. check full flag
-5. RESET is triggered
-6. wait and turn off RESET
-7.set RD is high
-8. reapeat step 7 depth times
-9. check empty flag
-10. check full-flag and empty-flag are high</t>
-  </si>
-  <si>
-    <t>tc_14</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_14</t>
-  </si>
-  <si>
-    <t>syn_fifo_tc_14.sv</t>
+2. write full data
+3. RESET
+4. write full data and check full flag
+5. read data and check empty flag</t>
+  </si>
+  <si>
+    <t>tc_11</t>
+  </si>
+  <si>
+    <t>syn_fifo_tc_11</t>
+  </si>
+  <si>
+    <t>syn_fifo_tc_11.sv</t>
   </si>
   <si>
     <t>Unexpected reset</t>
   </si>
   <si>
     <t>1. wait RESET
-2. set DATA IN and WR is high
-3. repeat step 2 with depth/2 times
-4. check full flag
-5. RESET is triggered
-6. wait and turn off RESET
-7.set RD is high
-8. reapeat step 7 depth/2 times
-9. check empty flag
-10. check full-flag and empty-flag are low and high</t>
+2. write half full data
+3. RESET
+4. write full data and check full flag
+5. read data and check empty flag</t>
   </si>
 </sst>
 </file>
@@ -589,7 +573,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +608,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1016,7 +1008,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1069,6 +1061,123 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1194,137 +1303,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1412,7 +1521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1421,19 +1530,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1445,38 +1575,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2029,116 +2207,116 @@
   </cols>
   <sheetData>
     <row r="2" ht="22.8" spans="2:7">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
     </row>
     <row r="3" ht="39" customHeight="1" spans="2:7">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="72" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" ht="16.8" spans="2:7">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="74" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" ht="16.8" spans="2:7">
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51" t="s">
+      <c r="B5" s="73"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="74" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" ht="16.8" spans="2:7">
-      <c r="B6" s="50"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51" t="s">
+      <c r="B6" s="73"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="51" t="s">
+      <c r="G6" s="74" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" ht="16.8" spans="2:7">
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="G7" s="74" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" ht="16.8" spans="2:7">
-      <c r="B8" s="50"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51" t="s">
+      <c r="B8" s="73"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="51" t="s">
+      <c r="F8" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="74" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2154,13 +2332,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:H43"/>
+  <dimension ref="B2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12:K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="20.2222222222222" customWidth="1"/>
     <col min="4" max="4" width="49.6666666666667" customWidth="1"/>
@@ -2170,7 +2348,7 @@
     <col min="8" max="8" width="13.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="21" spans="2:8">
+    <row r="2" ht="23.4" spans="2:11">
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
@@ -2192,569 +2370,692 @@
       <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" ht="23" customHeight="1" spans="2:8">
+      <c r="I2" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
+    </row>
+    <row r="3" ht="23" customHeight="1" spans="2:11">
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-    </row>
-    <row r="4" ht="18" spans="2:8">
+      <c r="I3" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" ht="18" spans="2:11">
       <c r="B4" s="8"/>
       <c r="C4" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-    </row>
-    <row r="5" ht="72" spans="2:8">
+      <c r="I4" s="58"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="60"/>
+    </row>
+    <row r="5" ht="72" spans="2:11">
       <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" ht="57.6" spans="2:8">
+        <v>27</v>
+      </c>
+      <c r="I5" s="55"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="57"/>
+    </row>
+    <row r="6" ht="57.6" spans="2:11">
       <c r="B6" s="20">
         <v>2</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
       <c r="H6" s="25"/>
-    </row>
-    <row r="7" ht="21" spans="2:8">
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="60"/>
+    </row>
+    <row r="7" ht="21" spans="2:11">
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="7"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-    </row>
-    <row r="8" ht="57.6" spans="2:8">
+      <c r="I7" s="61"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="63"/>
+    </row>
+    <row r="8" ht="57.6" spans="2:11">
       <c r="B8" s="20">
         <v>3</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F8" s="28" t="str">
         <f>"syn_fifo_"&amp;E8</f>
         <v>syn_fifo_tc_02</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="29"/>
-    </row>
-    <row r="9" ht="86.4" spans="2:8">
+        <v>34</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="55"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
+    </row>
+    <row r="9" ht="86.4" spans="2:11">
       <c r="B9" s="20">
         <v>4</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
-      <c r="H9" s="29"/>
-    </row>
-    <row r="10" ht="86.4" spans="2:8">
+      <c r="H9" s="32"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="66"/>
+    </row>
+    <row r="10" ht="86.4" spans="2:11">
       <c r="B10" s="20">
         <v>5</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="29"/>
-    </row>
-    <row r="11" ht="100.8" spans="2:8">
-      <c r="B11" s="20">
+        <v>38</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="60"/>
+    </row>
+    <row r="11" ht="72" spans="2:11">
+      <c r="B11" s="33">
         <v>6</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="27" t="s">
+      <c r="C11" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="D11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="E11" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="34"/>
-    </row>
-    <row r="12" ht="100.8" spans="2:8">
-      <c r="B12" s="20">
+      <c r="F11" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="68"/>
+      <c r="K11" s="69"/>
+    </row>
+    <row r="12" ht="100.8" spans="2:11">
+      <c r="B12" s="33">
         <v>7</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="34"/>
-    </row>
-    <row r="13" ht="72" spans="2:8">
-      <c r="B13" s="20">
+        <v>46</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="57"/>
+    </row>
+    <row r="13" ht="100.8" spans="2:11">
+      <c r="B13" s="33">
         <v>8</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="35"/>
-    </row>
-    <row r="14" ht="72" spans="2:8">
-      <c r="B14" s="20">
+        <v>51</v>
+      </c>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="66"/>
+    </row>
+    <row r="14" ht="72" spans="2:11">
+      <c r="B14" s="33">
         <v>9</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="36"/>
-    </row>
-    <row r="15" ht="72" spans="2:8">
-      <c r="B15" s="20">
+        <v>53</v>
+      </c>
+      <c r="E14" s="41"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="60"/>
+    </row>
+    <row r="15" ht="72" spans="2:11">
+      <c r="B15" s="33">
         <v>10</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="36"/>
-    </row>
-    <row r="16" ht="72" spans="2:8">
-      <c r="B16" s="20">
+        <v>55</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="55"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="57"/>
+    </row>
+    <row r="16" ht="72" spans="2:11">
+      <c r="B16" s="33">
         <v>11</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
+        <v>60</v>
+      </c>
+      <c r="E16" s="39"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
       <c r="H16" s="36"/>
-    </row>
-    <row r="17" ht="72" spans="2:8">
-      <c r="B17" s="20">
+      <c r="I16" s="64"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="66"/>
+    </row>
+    <row r="17" ht="72" spans="2:11">
+      <c r="B17" s="33">
         <v>12</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
+        <v>62</v>
+      </c>
+      <c r="E17" s="39"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="36"/>
-    </row>
-    <row r="18" ht="57.6" spans="2:8">
-      <c r="B18" s="20">
+      <c r="I17" s="58"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="60"/>
+    </row>
+    <row r="18" ht="57.6" spans="2:11">
+      <c r="B18" s="33">
         <v>13</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="36"/>
-    </row>
-    <row r="19" ht="28.8" spans="2:8">
-      <c r="B19" s="20">
+        <v>64</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="55"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="57"/>
+    </row>
+    <row r="19" ht="28.8" spans="2:11">
+      <c r="B19" s="33">
         <v>14</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
+        <v>69</v>
+      </c>
+      <c r="E19" s="39"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
       <c r="H19" s="36"/>
-    </row>
-    <row r="20" ht="72" spans="2:8">
-      <c r="B20" s="20">
+      <c r="I19" s="64"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="66"/>
+    </row>
+    <row r="20" ht="72" spans="2:11">
+      <c r="B20" s="33">
         <v>15</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
+        <v>71</v>
+      </c>
+      <c r="E20" s="39"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
       <c r="H20" s="36"/>
-    </row>
-    <row r="21" ht="100.8" spans="2:8">
-      <c r="B21" s="20">
+      <c r="I20" s="64"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="66"/>
+    </row>
+    <row r="21" ht="100.8" spans="2:11">
+      <c r="B21" s="33">
         <v>16</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
+        <v>73</v>
+      </c>
+      <c r="E21" s="41"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="36"/>
-    </row>
-    <row r="22" ht="115.2" spans="2:8">
-      <c r="B22" s="20">
+      <c r="I21" s="58"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="60"/>
+    </row>
+    <row r="22" ht="115.2" spans="2:11">
+      <c r="B22" s="33">
         <v>17</v>
       </c>
-      <c r="C22" s="37" t="s">
-        <v>68</v>
+      <c r="C22" s="44" t="s">
+        <v>74</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="H22" s="36"/>
-    </row>
-    <row r="23" ht="129.6" spans="2:8">
-      <c r="B23" s="20">
+        <v>75</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="55"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
+    </row>
+    <row r="23" ht="129.6" spans="2:11">
+      <c r="B23" s="33">
         <v>18</v>
       </c>
-      <c r="C23" s="38" t="s">
-        <v>73</v>
+      <c r="C23" s="45" t="s">
+        <v>79</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
+        <v>80</v>
+      </c>
+      <c r="E23" s="41"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
       <c r="H23" s="36"/>
-    </row>
-    <row r="24" ht="72" spans="2:8">
-      <c r="B24" s="20">
+      <c r="I23" s="58"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="60"/>
+    </row>
+    <row r="24" ht="72" spans="2:11">
+      <c r="B24" s="33">
         <v>19</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="H24" s="36"/>
-    </row>
-    <row r="25" ht="72" spans="2:8">
-      <c r="B25" s="20">
+        <v>82</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="55"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="57"/>
+    </row>
+    <row r="25" ht="72" spans="2:11">
+      <c r="B25" s="33">
         <v>20</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="36"/>
-    </row>
-    <row r="26" ht="43.2" spans="2:8">
-      <c r="B26" s="20">
+        <v>87</v>
+      </c>
+      <c r="E25" s="39"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="66"/>
+    </row>
+    <row r="26" ht="72" spans="2:11">
+      <c r="B26" s="33">
         <v>21</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="H26" s="34"/>
-    </row>
-    <row r="27" ht="43.2" spans="2:8">
-      <c r="B27" s="20">
+        <v>89</v>
+      </c>
+      <c r="E26" s="39"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="66"/>
+    </row>
+    <row r="27" ht="57.6" spans="2:11">
+      <c r="B27" s="33">
         <v>22</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
-    </row>
-    <row r="28" ht="21" spans="2:8">
+        <v>91</v>
+      </c>
+      <c r="E27" s="41"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="60"/>
+    </row>
+    <row r="28" ht="21" spans="2:11">
       <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="7"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-    </row>
-    <row r="29" ht="57.6" spans="2:8">
+      <c r="I28" s="61"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="63"/>
+    </row>
+    <row r="29" ht="57.6" spans="2:11">
       <c r="B29" s="20">
-        <v>22</v>
-      </c>
-      <c r="C29" s="39" t="s">
-        <v>90</v>
+        <v>23</v>
+      </c>
+      <c r="C29" s="46" t="s">
+        <v>93</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G29" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="H29" s="40"/>
-    </row>
-    <row r="30" ht="57.6" spans="2:8">
+        <v>97</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="55"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="57"/>
+    </row>
+    <row r="30" ht="57.6" spans="2:11">
       <c r="B30" s="20">
-        <v>23</v>
-      </c>
-      <c r="C30" s="41"/>
+        <v>24</v>
+      </c>
+      <c r="C30" s="47"/>
       <c r="D30" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="35"/>
-    </row>
-    <row r="31" ht="57.6" spans="2:8">
+        <v>98</v>
+      </c>
+      <c r="E30" s="30"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66"/>
+    </row>
+    <row r="31" ht="57.6" spans="2:11">
       <c r="B31" s="20">
-        <v>24</v>
-      </c>
-      <c r="C31" s="39" t="s">
-        <v>96</v>
+        <v>25</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>99</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="G31" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="H31" s="40"/>
-    </row>
-    <row r="32" ht="57.6" spans="2:8">
+      <c r="E31" s="30"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="66"/>
+    </row>
+    <row r="32" ht="57.6" spans="2:11">
       <c r="B32" s="20">
-        <v>25</v>
-      </c>
-      <c r="C32" s="42"/>
+        <v>26</v>
+      </c>
+      <c r="C32" s="48"/>
       <c r="D32" s="26" t="s">
         <v>101</v>
       </c>
       <c r="E32" s="30"/>
       <c r="F32" s="31"/>
       <c r="G32" s="31"/>
-      <c r="H32" s="34"/>
-    </row>
-    <row r="33" ht="57.6" spans="2:8">
+      <c r="H32" s="32"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="66"/>
+    </row>
+    <row r="33" ht="57.6" spans="2:11">
       <c r="B33" s="20">
-        <v>26</v>
-      </c>
-      <c r="C33" s="42"/>
+        <v>27</v>
+      </c>
+      <c r="C33" s="48"/>
       <c r="D33" s="26" t="s">
         <v>102</v>
       </c>
       <c r="E33" s="30"/>
       <c r="F33" s="31"/>
       <c r="G33" s="31"/>
-      <c r="H33" s="34"/>
-    </row>
-    <row r="34" ht="57.6" spans="2:8">
+      <c r="H33" s="32"/>
+      <c r="I33" s="64"/>
+      <c r="J33" s="65"/>
+      <c r="K33" s="66"/>
+    </row>
+    <row r="34" ht="57.6" spans="2:11">
       <c r="B34" s="20">
-        <v>27</v>
-      </c>
-      <c r="C34" s="41"/>
+        <v>28</v>
+      </c>
+      <c r="C34" s="47"/>
       <c r="D34" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="32"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="35"/>
-    </row>
-    <row r="35" ht="129.6" spans="2:8">
+      <c r="E34" s="49"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="59"/>
+      <c r="K34" s="60"/>
+    </row>
+    <row r="35" ht="129.6" spans="2:11">
       <c r="B35" s="20">
-        <v>28</v>
-      </c>
-      <c r="C35" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="44" t="s">
         <v>104</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="F35" s="28" t="s">
+      <c r="F35" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="G35" s="28" t="s">
+      <c r="G35" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="H35" s="40"/>
-    </row>
-    <row r="36" ht="86.4" spans="2:8">
+      <c r="H35" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I35" s="55"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="57"/>
+    </row>
+    <row r="36" ht="86.4" spans="2:11">
       <c r="B36" s="20">
-        <v>29</v>
-      </c>
-      <c r="C36" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="44" t="s">
         <v>109</v>
       </c>
       <c r="D36" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="35"/>
-    </row>
-    <row r="37" ht="57.6" spans="2:8">
+      <c r="E36" s="41"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="59"/>
+      <c r="K36" s="60"/>
+    </row>
+    <row r="37" ht="57.6" spans="2:11">
       <c r="B37" s="20">
-        <v>30</v>
-      </c>
-      <c r="C37" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="46" t="s">
         <v>111</v>
       </c>
       <c r="D37" s="26" t="s">
@@ -2769,164 +3070,188 @@
       <c r="G37" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="H37" s="40"/>
-    </row>
-    <row r="38" ht="43.2" spans="2:8">
+      <c r="H37" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37" s="55"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="57"/>
+    </row>
+    <row r="38" ht="43.2" spans="2:11">
       <c r="B38" s="20">
-        <v>31</v>
-      </c>
-      <c r="C38" s="41"/>
+        <v>32</v>
+      </c>
+      <c r="C38" s="47"/>
       <c r="D38" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="E38" s="32"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="35"/>
-    </row>
-    <row r="39" ht="72" spans="2:8">
+      <c r="E38" s="30"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="66"/>
+    </row>
+    <row r="39" ht="72" spans="2:11">
       <c r="B39" s="20">
-        <v>32</v>
-      </c>
-      <c r="C39" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="46" t="s">
         <v>117</v>
       </c>
       <c r="D39" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="30"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="64"/>
+      <c r="J39" s="65"/>
+      <c r="K39" s="66"/>
+    </row>
+    <row r="40" ht="57.6" spans="2:11">
+      <c r="B40" s="20">
+        <v>34</v>
+      </c>
+      <c r="C40" s="47"/>
+      <c r="D40" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="F39" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="G39" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="H39" s="40"/>
-    </row>
-    <row r="40" ht="57.6" spans="2:8">
-      <c r="B40" s="20">
-        <v>33</v>
-      </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="E40" s="32"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="35"/>
-    </row>
-    <row r="41" ht="21" spans="2:8">
+      <c r="E40" s="49"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="58"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="60"/>
+    </row>
+    <row r="41" ht="21" spans="2:11">
       <c r="B41" s="4"/>
       <c r="C41" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="7"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
-    </row>
-    <row r="42" ht="144" spans="2:8">
+      <c r="I41" s="61"/>
+      <c r="J41" s="62"/>
+      <c r="K41" s="63"/>
+    </row>
+    <row r="42" ht="72" spans="2:11">
       <c r="B42" s="20">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C42" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="E42" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="F42" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="D42" s="26" t="s">
+      <c r="G42" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="E42" s="43" t="s">
+      <c r="H42" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I42" s="55"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="57"/>
+    </row>
+    <row r="43" ht="72" spans="2:11">
+      <c r="B43" s="20">
+        <v>36</v>
+      </c>
+      <c r="C43" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="F42" s="44" t="s">
+      <c r="D43" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="G42" s="44" t="s">
-        <v>128</v>
-      </c>
-      <c r="H42" s="40"/>
-    </row>
-    <row r="43" ht="144" spans="2:8">
-      <c r="B43" s="20">
-        <v>35</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="D43" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="E43" s="45"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="46"/>
-      <c r="H43" s="35"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="59"/>
+      <c r="K43" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="65">
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I41:K41"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="C31:C34"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="E15:E17"/>
     <mergeCell ref="E18:E21"/>
     <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="E29:E34"/>
     <mergeCell ref="E35:E36"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="E37:E40"/>
     <mergeCell ref="E42:E43"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="F8:F10"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F15:F17"/>
     <mergeCell ref="F18:F21"/>
     <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="F29:F34"/>
     <mergeCell ref="F35:F36"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F37:F40"/>
     <mergeCell ref="F42:F43"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="G8:G10"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G15:G17"/>
     <mergeCell ref="G18:G21"/>
     <mergeCell ref="G22:G23"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="G29:G34"/>
     <mergeCell ref="G35:G36"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="G37:G40"/>
     <mergeCell ref="G42:G43"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="H8:H10"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="H15:H17"/>
     <mergeCell ref="H18:H21"/>
     <mergeCell ref="H22:H23"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="H31:H34"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H29:H34"/>
     <mergeCell ref="H35:H36"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H37:H40"/>
     <mergeCell ref="H42:H43"/>
+    <mergeCell ref="I3:K4"/>
+    <mergeCell ref="I5:K6"/>
+    <mergeCell ref="I8:K10"/>
+    <mergeCell ref="I12:K14"/>
+    <mergeCell ref="I15:K17"/>
+    <mergeCell ref="I18:K21"/>
+    <mergeCell ref="I22:K23"/>
+    <mergeCell ref="I24:K27"/>
+    <mergeCell ref="I29:K34"/>
+    <mergeCell ref="I35:K36"/>
+    <mergeCell ref="I37:K40"/>
+    <mergeCell ref="I42:K43"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H6 H8:H27 H29:H40 H42:H43">

</xml_diff>